<commit_message>
Update CAFEData interface with department options
</commit_message>
<xml_diff>
--- a/test_cases/cafe-data-interface-test-cases.xlsx
+++ b/test_cases/cafe-data-interface-test-cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\cis315_OfficeHours\test_cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\cis315_OfficeHours\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Test Number</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>8-9 run as single unit test</t>
+  </si>
+  <si>
+    <t>Retrieve list of all departments of type department and populate string list and check count</t>
+  </si>
+  <si>
+    <t>Retrieve a list of faculty for Chemistry department searching on the string Chemistry and check count</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,10 +465,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="D2">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
@@ -636,6 +642,40 @@
         <v>16</v>
       </c>
       <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>